<commit_message>
"thêm show details DC và sửa date trong tableview "
</commit_message>
<xml_diff>
--- a/MedicineManagement/save/QLTuThuoc.xlsx
+++ b/MedicineManagement/save/QLTuThuoc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TuThuoc-SceneBuilder\MedicineManagement\save\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B953C040-E8BE-408F-9360-D3C809C1034D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A17E6B7-FC8B-4843-96C1-EA6DE26B5003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MEDICINE" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="59">
   <si>
     <t>ID</t>
   </si>
@@ -122,36 +122,18 @@
     <t>Use</t>
   </si>
   <si>
-    <t>Nhiet ke dien tu</t>
-  </si>
-  <si>
     <t>Chiec</t>
   </si>
   <si>
     <t>Do than nhiet</t>
   </si>
   <si>
-    <t>Nhiet ke hong ngoai</t>
-  </si>
-  <si>
-    <t>May do nong do oxy</t>
-  </si>
-  <si>
     <t>Do nong do oxy trong mau</t>
   </si>
   <si>
-    <t>Bang ca nhan</t>
-  </si>
-  <si>
     <t>Bang dan bao ve vet thuong</t>
   </si>
   <si>
-    <t>Bang gac</t>
-  </si>
-  <si>
-    <t>Dung sat trung vet thuong</t>
-  </si>
-  <si>
     <t>Paracetamol</t>
   </si>
   <si>
@@ -207,6 +189,30 @@
   </si>
   <si>
     <t>Lieu</t>
+  </si>
+  <si>
+    <t>Toa Thuoc so 2</t>
+  </si>
+  <si>
+    <t>2 lan 1 ngay</t>
+  </si>
+  <si>
+    <t>Nhiệt kế điện tử Pharmacity</t>
+  </si>
+  <si>
+    <t>Nhiệt kế hồng ngoại Urgo</t>
+  </si>
+  <si>
+    <t>Máy đo nồng độ oxy trong máu iMedicare iOM-A8</t>
+  </si>
+  <si>
+    <t>Băng dán có gạc Urgosterile </t>
+  </si>
+  <si>
+    <t>Dụng cụ xét nghiệm nhanh Covid-19 Antigen Self-Test Abbott Panbio Test Kit</t>
+  </si>
+  <si>
+    <t>Test Covid</t>
   </si>
 </sst>
 </file>
@@ -216,7 +222,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -232,6 +238,13 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -255,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -263,6 +276,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,7 +539,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -545,7 +559,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -585,7 +599,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -605,7 +619,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -645,7 +659,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -685,7 +699,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -705,7 +719,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -725,16 +739,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C12">
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F12" s="3">
         <v>44772</v>
@@ -751,9 +765,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
@@ -768,13 +782,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -782,13 +796,27 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C2" s="4">
         <v>44749</v>
       </c>
       <c r="D2" s="4">
         <v>44757</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="4">
+        <v>44754</v>
+      </c>
+      <c r="D3" s="4">
+        <v>44751</v>
       </c>
     </row>
   </sheetData>
@@ -865,7 +893,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13:XFD14"/>
@@ -875,19 +903,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D1" t="s">
-        <v>56</v>
-      </c>
       <c r="E1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
@@ -895,7 +923,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -912,7 +940,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -946,7 +974,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -963,7 +991,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
@@ -997,7 +1025,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -1031,7 +1059,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -1048,7 +1076,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -1065,16 +1093,33 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E12">
         <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1090,11 +1135,15 @@
   </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="66.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1113,63 +1162,63 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
         <v>28</v>
       </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="E2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
         <v>29</v>
       </c>
-      <c r="E3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -1178,27 +1227,28 @@
         <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>37</v>
+      <c r="D6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
"Thêm thông báo và màu mè cho tableview tủ thuốc"
</commit_message>
<xml_diff>
--- a/MedicineManagement/save/QLTuThuoc.xlsx
+++ b/MedicineManagement/save/QLTuThuoc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TuThuoc-SceneBuilder\MedicineManagement\save\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A17E6B7-FC8B-4843-96C1-EA6DE26B5003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F39739-5ADE-418F-9948-78EDBB74B008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MEDICINE" sheetId="1" r:id="rId1"/>
@@ -767,8 +767,8 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -816,7 +816,8 @@
         <v>44754</v>
       </c>
       <c r="D3" s="4">
-        <v>44751</v>
+        <f>DATE(2022,7,7)</f>
+        <v>44749</v>
       </c>
     </row>
   </sheetData>
@@ -1135,7 +1136,7 @@
   </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>

</xml_diff>